<commit_message>
added a routine to plot both the undamaged and the ocmplete dataset
</commit_message>
<xml_diff>
--- a/indentation/caracterization/tiguida/tensile_testings_porks/parameters_Yeoh_Mooney.xlsx
+++ b/indentation/caracterization/tiguida/tensile_testings_porks/parameters_Yeoh_Mooney.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siaquinta\Documents\Projet Périnée\perineal_indentation\indentation\caracterization\tiguida\tensile_testings_porks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D099BC46-EBDC-4A98-878E-CA3D2661A6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB5972D-AE4C-4E32-B6CF-D44131DDE763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{F231E33D-BB98-4446-B9A8-A9D10947690E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F231E33D-BB98-4446-B9A8-A9D10947690E}"/>
   </bookViews>
   <sheets>
     <sheet name="Yeoh" sheetId="1" r:id="rId1"/>
@@ -184,15 +184,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>561048</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152310</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>218148</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -215,7 +215,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4572000" y="952500"/>
+          <a:off x="4991100" y="742950"/>
           <a:ext cx="7419048" cy="723810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F84AD4C-8A61-4D8F-9113-259567A97A46}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,350 +600,173 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>210.60154159000001</v>
-      </c>
-      <c r="C2">
-        <v>525.22251811000001</v>
-      </c>
-      <c r="D2">
-        <v>-1893.02162041</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>153.86785194999999</v>
-      </c>
-      <c r="C3">
-        <v>-169.37808759000001</v>
-      </c>
-      <c r="D3">
-        <v>7340.3232790299999</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>70.411186909999998</v>
+        <v>82</v>
       </c>
       <c r="C4">
-        <v>443.98448538999997</v>
+        <v>320</v>
       </c>
       <c r="D4">
-        <v>-128.51587986000001</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>15.76751795</v>
-      </c>
-      <c r="C5">
-        <v>20.981834159999998</v>
-      </c>
-      <c r="D5">
-        <v>-0.17382679000000001</v>
-      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>242.90944952000001</v>
-      </c>
-      <c r="C6">
-        <v>127.97922694</v>
-      </c>
-      <c r="D6">
-        <v>-127.00997448</v>
-      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
-        <v>82.1997152</v>
-      </c>
-      <c r="C7">
-        <v>363.00247109999998</v>
-      </c>
-      <c r="D7">
-        <v>-541.08390357999997</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>26.919093310000001</v>
-      </c>
-      <c r="C8">
-        <v>338.93808970999999</v>
-      </c>
-      <c r="D8">
-        <v>-145.52536663000001</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>38.14114197</v>
+        <v>96</v>
       </c>
       <c r="C9">
-        <v>187.25421674</v>
+        <v>127</v>
       </c>
       <c r="D9">
-        <v>-51.61170087</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>13.30231551</v>
-      </c>
-      <c r="C10">
-        <v>33.803780619999998</v>
-      </c>
-      <c r="D10">
-        <v>-1.38450896</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>183.51765900000001</v>
-      </c>
-      <c r="C11" s="1">
-        <v>12578.6877</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-513009.12699999998</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>145.14235484</v>
-      </c>
-      <c r="C12">
-        <v>224.88231615000001</v>
-      </c>
-      <c r="D12">
-        <v>-295.25359671000001</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
-        <v>20.361541089999999</v>
-      </c>
-      <c r="C13">
-        <v>-2.2579303199999998</v>
-      </c>
-      <c r="D13">
-        <v>2.8807515700000002</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>47.123735490000001</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>135.69273161999999</v>
+        <v>127</v>
       </c>
       <c r="D14">
-        <v>-15.65280147</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
-        <v>25.822906799999998</v>
-      </c>
-      <c r="C15">
-        <v>50.739814199999998</v>
-      </c>
-      <c r="D15">
-        <v>-0.33483688</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>205.876262</v>
-      </c>
-      <c r="C16">
-        <v>381.25074675000002</v>
-      </c>
-      <c r="D16">
-        <v>-347.06559912</v>
-      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
-        <v>136.43682745999999</v>
-      </c>
-      <c r="C17">
-        <v>545.77804037999999</v>
-      </c>
-      <c r="D17">
-        <v>-451.27605725000001</v>
-      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>55.522638479999998</v>
-      </c>
-      <c r="C18">
-        <v>21.957645719999999</v>
-      </c>
-      <c r="D18">
-        <v>-2.5983537000000001</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>33.562626309999999</v>
+        <v>46</v>
       </c>
       <c r="C19">
-        <v>156.29291502000001</v>
+        <v>118</v>
       </c>
       <c r="D19">
-        <v>1.0393372599999999</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
-        <v>7.1125895000000003</v>
-      </c>
-      <c r="C20">
-        <v>8.5756101900000008</v>
-      </c>
-      <c r="D20">
-        <v>-0.92244999999999999</v>
-      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>219.65958022999999</v>
-      </c>
-      <c r="C21">
-        <v>760.60701620999998</v>
-      </c>
-      <c r="D21">
-        <v>-799.55025688000001</v>
-      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>226.29627219</v>
-      </c>
-      <c r="C22">
-        <v>292.47322076</v>
-      </c>
-      <c r="D22">
-        <v>-555.00600801999997</v>
-      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>22.90496096</v>
-      </c>
-      <c r="C23">
-        <v>47.106164999999997</v>
-      </c>
-      <c r="D23">
-        <v>-9.5386786800000003</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>28.87320222</v>
+        <v>46</v>
       </c>
       <c r="C24">
-        <v>324.87246045000001</v>
+        <v>252</v>
       </c>
       <c r="D24">
-        <v>-44.764868970000002</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
-        <v>17.87646724</v>
-      </c>
-      <c r="C25">
-        <v>42.219847510000001</v>
-      </c>
-      <c r="D25">
-        <v>-12.839895</v>
-      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
-      </c>
-      <c r="B26">
-        <v>345.11844042000001</v>
-      </c>
-      <c r="C26">
-        <v>1508.26752816</v>
-      </c>
-      <c r="D26">
-        <v>-2119.3901684399998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>